<commit_message>
Sync + Materi B.Indo
</commit_message>
<xml_diff>
--- a/Roster Ujian Mid Ganjil.xlsx
+++ b/Roster Ujian Mid Ganjil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Repositories\Beethoven-Class-IX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0D7FFF-2ED8-4A16-8696-2B03069A328A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659265E7-E4E1-4BB7-8244-D3460554B192}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="18000" windowHeight="9360" xr2:uid="{324D93F8-1E7F-42D4-9E04-B5D52CD7C9C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{324D93F8-1E7F-42D4-9E04-B5D52CD7C9C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>ROSTER UJIAN MID SEMESTER GANJIL</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>B. ING</t>
+  </si>
+  <si>
+    <t>✔️</t>
   </si>
 </sst>
 </file>
@@ -241,6 +244,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -248,21 +266,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -582,7 +585,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E3" sqref="A3:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,22 +598,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -630,7 +633,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -639,22 +642,30 @@
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -663,11 +674,13 @@
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -678,7 +691,7 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -691,7 +704,7 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
@@ -702,7 +715,7 @@
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -715,7 +728,7 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -726,20 +739,20 @@
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
@@ -750,31 +763,35 @@
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -787,11 +804,11 @@
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="2"/>

</xml_diff>